<commit_message>
fixed example species name in HV xlsx data template
</commit_message>
<xml_diff>
--- a/protocols/HerbVar Datasheet Template.xlsx
+++ b/protocols/HerbVar Datasheet Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick.lyon/Documents/Jobs/2021_HerbVar Network Admin/Phase 2 Protocol Revision/Datasheet Edits/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamwetzel/Repos/HerbVar.github.io/protocols/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E30303-275A-4846-B28A-FCC6B0F82BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D33A98-36E5-474E-851F-5B5056ECA044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37000" yWindow="2780" windowWidth="30700" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="siteData" sheetId="1" r:id="rId1"/>
@@ -546,9 +546,6 @@
   </si>
   <si>
     <t>percLf30</t>
-  </si>
-  <si>
-    <t>e.g., Plantago_major</t>
   </si>
   <si>
     <t>e.g., Plantago</t>
@@ -1374,6 +1371,9 @@
   </si>
   <si>
     <t>columnName</t>
+  </si>
+  <si>
+    <t>e.g., major</t>
   </si>
 </sst>
 </file>
@@ -2294,9 +2294,9 @@
   </sheetPr>
   <dimension ref="A1:BZ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2403,7 +2403,7 @@
       <c r="B2" s="113"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3" t="s">
-        <v>162</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:78" ht="13" x14ac:dyDescent="0.15">
@@ -2413,7 +2413,7 @@
       <c r="B3" s="113"/>
       <c r="C3" s="1"/>
       <c r="D3" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:78" ht="13" x14ac:dyDescent="0.15">
@@ -2433,7 +2433,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:78" ht="13" x14ac:dyDescent="0.15">
@@ -2445,7 +2445,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:78" ht="13" x14ac:dyDescent="0.15">
@@ -2506,10 +2506,10 @@
       </c>
       <c r="B11" s="114"/>
       <c r="C11" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E11" s="112"/>
     </row>
@@ -2547,7 +2547,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E14" s="112"/>
     </row>
@@ -2645,7 +2645,7 @@
         <v>114</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2683,7 +2683,7 @@
         <v>112</v>
       </c>
       <c r="B1" s="68" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C1" s="69" t="s">
         <v>2</v>
@@ -2703,7 +2703,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="66" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="75" customFormat="1" ht="14" x14ac:dyDescent="0.15">
@@ -2717,7 +2717,7 @@
         <v>80</v>
       </c>
       <c r="D3" s="74" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2731,7 +2731,7 @@
         <v>80</v>
       </c>
       <c r="D4" s="66" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="75" customFormat="1" ht="14" x14ac:dyDescent="0.15">
@@ -2745,7 +2745,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="74" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28" x14ac:dyDescent="0.15">
@@ -2759,7 +2759,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="66" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="75" customFormat="1" ht="14" x14ac:dyDescent="0.15">
@@ -2826,10 +2826,10 @@
         <v>84</v>
       </c>
       <c r="C11" s="74" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D11" s="74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2970,7 +2970,7 @@
     </row>
     <row r="21" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" s="71" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B21" s="50" t="s">
         <v>107</v>
@@ -2979,12 +2979,12 @@
         <v>75</v>
       </c>
       <c r="D21" s="89" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:46" s="75" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="73" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B22" s="45" t="s">
         <v>106</v>
@@ -2993,26 +2993,26 @@
         <v>75</v>
       </c>
       <c r="D22" s="90" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="71" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B23" s="63" t="s">
         <v>59</v>
       </c>
       <c r="C23" s="89" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D23" s="89" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:46" s="75" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A24" s="73" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B24" s="44" t="s">
         <v>97</v>
@@ -3021,18 +3021,18 @@
         <v>5</v>
       </c>
       <c r="D24" s="90" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A25" s="71" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B25" s="63" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="66" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:46" s="88" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -3052,7 +3052,7 @@
         <v>63</v>
       </c>
       <c r="D27" s="89" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:46" s="75" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -3066,7 +3066,7 @@
         <v>61</v>
       </c>
       <c r="D28" s="74" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:46" ht="28" x14ac:dyDescent="0.15">
@@ -3080,7 +3080,7 @@
         <v>64</v>
       </c>
       <c r="D29" s="89" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:46" s="75" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -3094,7 +3094,7 @@
         <v>63</v>
       </c>
       <c r="D30" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:46" ht="14" x14ac:dyDescent="0.15">
@@ -3147,7 +3147,7 @@
         <v>62</v>
       </c>
       <c r="B34" s="52" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C34" s="76" t="s">
         <v>78</v>
@@ -3170,7 +3170,7 @@
         <v>67</v>
       </c>
       <c r="D35" s="66" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AQ35" s="50"/>
       <c r="AR35" s="50"/>
@@ -3207,7 +3207,7 @@
         <v>69</v>
       </c>
       <c r="D37" s="66" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AO37" s="50"/>
       <c r="AP37" s="50"/>
@@ -3227,7 +3227,7 @@
         <v>72</v>
       </c>
       <c r="D38" s="74" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AN38" s="45"/>
       <c r="AO38" s="45"/>
@@ -3248,7 +3248,7 @@
         <v>73</v>
       </c>
       <c r="D39" s="66" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AM39" s="50"/>
       <c r="AN39" s="50"/>
@@ -3336,13 +3336,13 @@
         <v>62</v>
       </c>
       <c r="B43" s="49" t="s">
+        <v>228</v>
+      </c>
+      <c r="C43" s="97" t="s">
         <v>229</v>
       </c>
-      <c r="C43" s="97" t="s">
+      <c r="D43" s="89" t="s">
         <v>230</v>
-      </c>
-      <c r="D43" s="89" t="s">
-        <v>231</v>
       </c>
       <c r="AI43" s="50"/>
       <c r="AJ43" s="50"/>
@@ -3368,7 +3368,7 @@
         <v>75</v>
       </c>
       <c r="D44" s="74" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AH44" s="45"/>
       <c r="AI44" s="45"/>
@@ -3395,7 +3395,7 @@
         <v>67</v>
       </c>
       <c r="D45" s="66" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG45" s="50"/>
       <c r="AH45" s="50"/>
@@ -3423,7 +3423,7 @@
         <v>70</v>
       </c>
       <c r="D46" s="90" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AF46" s="45"/>
       <c r="AG46" s="45"/>
@@ -3448,10 +3448,10 @@
         <v>128</v>
       </c>
       <c r="C47" s="89" t="s">
+        <v>180</v>
+      </c>
+      <c r="D47" s="89" t="s">
         <v>181</v>
-      </c>
-      <c r="D47" s="89" t="s">
-        <v>182</v>
       </c>
       <c r="AE47" s="50"/>
       <c r="AF47" s="50"/>
@@ -3478,10 +3478,10 @@
         <v>129</v>
       </c>
       <c r="C48" s="98" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D48" s="90" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AD48" s="51"/>
       <c r="AE48" s="45"/>
@@ -3503,7 +3503,7 @@
     </row>
     <row r="49" spans="1:46" ht="56" x14ac:dyDescent="0.15">
       <c r="A49" s="71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B49" s="49" t="s">
         <v>130</v>
@@ -3512,7 +3512,7 @@
         <v>69</v>
       </c>
       <c r="D49" s="66" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P49" s="49"/>
       <c r="Q49" s="49"/>
@@ -3521,7 +3521,7 @@
     </row>
     <row r="50" spans="1:46" s="75" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A50" s="73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B50" s="52" t="s">
         <v>131</v>
@@ -3530,7 +3530,7 @@
         <v>69</v>
       </c>
       <c r="D50" s="74" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O50" s="52"/>
       <c r="P50" s="52"/>
@@ -3543,13 +3543,13 @@
         <v>62</v>
       </c>
       <c r="B51" s="49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C51" s="65" t="s">
         <v>67</v>
       </c>
       <c r="D51" s="66" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U51" s="48"/>
       <c r="V51" s="48"/>
@@ -3581,7 +3581,7 @@
         <v>80</v>
       </c>
       <c r="D52" s="74" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E52" s="52"/>
       <c r="F52" s="51"/>
@@ -3631,13 +3631,13 @@
         <v>62</v>
       </c>
       <c r="B53" s="50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C53" s="65" t="s">
         <v>67</v>
       </c>
       <c r="D53" s="66" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E53" s="50"/>
       <c r="F53" s="50"/>
@@ -3732,7 +3732,7 @@
     </row>
     <row r="55" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A55" s="71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B55" s="99" t="s">
         <v>18</v>
@@ -3741,12 +3741,12 @@
         <v>63</v>
       </c>
       <c r="D55" s="89" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:46" s="75" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A56" s="73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B56" s="55" t="s">
         <v>86</v>
@@ -3755,12 +3755,12 @@
         <v>63</v>
       </c>
       <c r="D56" s="74" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A57" s="71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B57" s="99" t="s">
         <v>11</v>
@@ -3769,12 +3769,12 @@
         <v>64</v>
       </c>
       <c r="D57" s="89" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:46" s="75" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A58" s="73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B58" s="55" t="s">
         <v>19</v>
@@ -3783,12 +3783,12 @@
         <v>63</v>
       </c>
       <c r="D58" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A59" s="71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B59" s="99" t="s">
         <v>20</v>
@@ -3797,12 +3797,12 @@
         <v>70</v>
       </c>
       <c r="D59" s="66" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="60" spans="1:46" s="75" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" s="73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B60" s="100" t="s">
         <v>44</v>
@@ -3816,35 +3816,35 @@
     </row>
     <row r="61" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A61" s="71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B61" s="101" t="s">
         <v>116</v>
       </c>
       <c r="C61" s="66" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D61" s="97" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62" spans="1:46" s="75" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A62" s="73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B62" s="100" t="s">
         <v>117</v>
       </c>
       <c r="C62" s="90" t="s">
+        <v>198</v>
+      </c>
+      <c r="D62" s="90" t="s">
         <v>199</v>
-      </c>
-      <c r="D62" s="90" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="63" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A63" s="71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B63" s="101" t="s">
         <v>45</v>
@@ -3858,7 +3858,7 @@
     </row>
     <row r="64" spans="1:46" s="75" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A64" s="73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B64" s="100" t="s">
         <v>46</v>
@@ -3867,12 +3867,12 @@
         <v>69</v>
       </c>
       <c r="D64" s="74" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A65" s="71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B65" s="99" t="s">
         <v>123</v>
@@ -3881,12 +3881,12 @@
         <v>69</v>
       </c>
       <c r="D65" s="89" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="66" spans="1:19" s="75" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B66" s="55" t="s">
         <v>124</v>
@@ -3895,12 +3895,12 @@
         <v>69</v>
       </c>
       <c r="D66" s="90" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="67" spans="1:19" ht="28" x14ac:dyDescent="0.15">
       <c r="A67" s="71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B67" s="99" t="s">
         <v>125</v>
@@ -3909,12 +3909,12 @@
         <v>69</v>
       </c>
       <c r="D67" s="89" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="68" spans="1:19" s="75" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A68" s="73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B68" s="55" t="s">
         <v>126</v>
@@ -3923,12 +3923,12 @@
         <v>69</v>
       </c>
       <c r="D68" s="90" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="70" x14ac:dyDescent="0.15">
       <c r="A69" s="71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B69" s="101" t="s">
         <v>47</v>
@@ -3937,12 +3937,12 @@
         <v>67</v>
       </c>
       <c r="D69" s="66" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="70" spans="1:19" s="75" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A70" s="73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B70" s="55" t="s">
         <v>134</v>
@@ -3951,12 +3951,12 @@
         <v>67</v>
       </c>
       <c r="D70" s="90" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="71" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A71" s="71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B71" s="99" t="s">
         <v>135</v>
@@ -3965,12 +3965,12 @@
         <v>67</v>
       </c>
       <c r="D71" s="89" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="72" spans="1:19" s="75" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A72" s="73" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B72" s="55" t="s">
         <v>136</v>
@@ -3979,12 +3979,12 @@
         <v>67</v>
       </c>
       <c r="D72" s="90" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="1:19" ht="28" x14ac:dyDescent="0.15">
       <c r="A73" s="71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B73" s="99" t="s">
         <v>137</v>
@@ -3993,26 +3993,26 @@
         <v>67</v>
       </c>
       <c r="D73" s="89" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" spans="1:19" s="75" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A74" s="73" t="s">
+        <v>188</v>
+      </c>
+      <c r="B74" s="100" t="s">
         <v>189</v>
-      </c>
-      <c r="B74" s="100" t="s">
-        <v>190</v>
       </c>
       <c r="C74" s="98" t="s">
         <v>67</v>
       </c>
       <c r="D74" s="74" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" spans="1:19" ht="28" x14ac:dyDescent="0.15">
       <c r="A75" s="71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B75" s="99" t="s">
         <v>3</v>
@@ -4021,7 +4021,7 @@
         <v>80</v>
       </c>
       <c r="D75" s="66" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="76" spans="1:19" s="88" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -4032,7 +4032,7 @@
     </row>
     <row r="77" spans="1:19" ht="28" x14ac:dyDescent="0.15">
       <c r="A77" s="71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B77" s="49" t="s">
         <v>18</v>
@@ -4041,12 +4041,12 @@
         <v>63</v>
       </c>
       <c r="D77" s="89" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="78" spans="1:19" s="75" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A78" s="73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B78" s="52" t="s">
         <v>86</v>
@@ -4055,12 +4055,12 @@
         <v>63</v>
       </c>
       <c r="D78" s="74" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="79" spans="1:19" ht="28" x14ac:dyDescent="0.15">
       <c r="A79" s="71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B79" s="49" t="s">
         <v>11</v>
@@ -4069,12 +4069,12 @@
         <v>64</v>
       </c>
       <c r="D79" s="89" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="80" spans="1:19" s="75" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A80" s="73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B80" s="52" t="s">
         <v>19</v>
@@ -4083,14 +4083,14 @@
         <v>63</v>
       </c>
       <c r="D80" s="90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R80" s="52"/>
       <c r="S80" s="51"/>
     </row>
     <row r="81" spans="1:28" ht="28" x14ac:dyDescent="0.15">
       <c r="A81" s="71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B81" s="49" t="s">
         <v>20</v>
@@ -4099,7 +4099,7 @@
         <v>70</v>
       </c>
       <c r="D81" s="66" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q81" s="49"/>
       <c r="R81" s="49"/>
@@ -4107,16 +4107,16 @@
     </row>
     <row r="82" spans="1:28" s="75" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A82" s="73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B82" s="52" t="s">
         <v>139</v>
       </c>
       <c r="C82" s="106" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D82" s="107" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N82" s="52"/>
       <c r="O82" s="52"/>
@@ -4127,7 +4127,7 @@
     </row>
     <row r="83" spans="1:28" ht="28" x14ac:dyDescent="0.15">
       <c r="A83" s="71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B83" s="49" t="s">
         <v>41</v>
@@ -4136,7 +4136,7 @@
         <v>69</v>
       </c>
       <c r="D83" s="66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M83" s="49"/>
       <c r="N83" s="49"/>
@@ -4148,7 +4148,7 @@
     </row>
     <row r="84" spans="1:28" s="75" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A84" s="73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B84" s="52" t="s">
         <v>132</v>
@@ -4157,7 +4157,7 @@
         <v>69</v>
       </c>
       <c r="D84" s="74" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L84" s="51"/>
       <c r="M84" s="52"/>
@@ -4170,7 +4170,7 @@
     </row>
     <row r="85" spans="1:28" ht="70" x14ac:dyDescent="0.15">
       <c r="A85" s="71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B85" s="49" t="s">
         <v>42</v>
@@ -4179,7 +4179,7 @@
         <v>69</v>
       </c>
       <c r="D85" s="66" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K85" s="48"/>
       <c r="L85" s="48"/>
@@ -4193,16 +4193,16 @@
     </row>
     <row r="86" spans="1:28" s="75" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A86" s="73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B86" s="52" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C86" s="74" t="s">
         <v>69</v>
       </c>
       <c r="D86" s="74" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K86" s="51"/>
       <c r="L86" s="51"/>
@@ -4216,7 +4216,7 @@
     </row>
     <row r="87" spans="1:28" ht="56" x14ac:dyDescent="0.15">
       <c r="A87" s="71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B87" s="49" t="s">
         <v>43</v>
@@ -4225,26 +4225,26 @@
         <v>69</v>
       </c>
       <c r="D87" s="66" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="1:28" s="75" customFormat="1" ht="84" x14ac:dyDescent="0.15">
       <c r="A88" s="73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B88" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C88" s="76" t="s">
         <v>69</v>
       </c>
       <c r="D88" s="74" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="89" spans="1:28" ht="56" x14ac:dyDescent="0.15">
       <c r="A89" s="71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B89" s="49" t="s">
         <v>133</v>
@@ -4253,26 +4253,26 @@
         <v>69</v>
       </c>
       <c r="D89" s="89" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="90" spans="1:28" s="75" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A90" s="73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B90" s="52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C90" s="76" t="s">
         <v>69</v>
       </c>
       <c r="D90" s="90" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="91" spans="1:28" ht="28" x14ac:dyDescent="0.15">
       <c r="A91" s="71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B91" s="49" t="s">
         <v>140</v>
@@ -4281,7 +4281,7 @@
         <v>69</v>
       </c>
       <c r="D91" s="89" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F91" s="108"/>
       <c r="G91" s="108"/>
@@ -4309,7 +4309,7 @@
     </row>
     <row r="92" spans="1:28" s="75" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A92" s="73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B92" s="52" t="s">
         <v>141</v>
@@ -4318,7 +4318,7 @@
         <v>69</v>
       </c>
       <c r="D92" s="90" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E92" s="53"/>
       <c r="F92" s="53"/>
@@ -4347,16 +4347,16 @@
     </row>
     <row r="93" spans="1:28" ht="56" x14ac:dyDescent="0.15">
       <c r="A93" s="71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B93" s="49" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C93" s="77" t="s">
         <v>69</v>
       </c>
       <c r="D93" s="89" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E93" s="108"/>
       <c r="F93" s="108"/>
@@ -4385,16 +4385,16 @@
     </row>
     <row r="94" spans="1:28" s="75" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A94" s="73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B94" s="52" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C94" s="74" t="s">
         <v>69</v>
       </c>
       <c r="D94" s="90" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E94" s="53"/>
       <c r="F94" s="53"/>
@@ -4423,7 +4423,7 @@
     </row>
     <row r="95" spans="1:28" ht="28" x14ac:dyDescent="0.15">
       <c r="A95" s="71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B95" s="49" t="s">
         <v>3</v>
@@ -4432,7 +4432,7 @@
         <v>80</v>
       </c>
       <c r="D95" s="66" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E95" s="108"/>
       <c r="F95" s="108"/>
@@ -4473,7 +4473,7 @@
         <v>143</v>
       </c>
       <c r="D97" s="89" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="13" x14ac:dyDescent="0.15"/>
@@ -4697,7 +4697,7 @@
         <v>20</v>
       </c>
       <c r="H1" s="52" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I1" s="52" t="s">
         <v>23</v>
@@ -4724,7 +4724,7 @@
         <v>28</v>
       </c>
       <c r="Q1" s="52" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="R1" s="51" t="s">
         <v>29</v>
@@ -4781,16 +4781,16 @@
         <v>3</v>
       </c>
       <c r="AJ1" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="AK1" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="AK1" s="52" t="s">
+      <c r="AL1" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="AL1" s="52" t="s">
+      <c r="AM1" s="52" t="s">
         <v>168</v>
-      </c>
-      <c r="AM1" s="52" t="s">
-        <v>169</v>
       </c>
       <c r="AN1" s="45" t="s">
         <v>146</v>
@@ -4864,10 +4864,10 @@
       <c r="K2" s="117"/>
       <c r="L2" s="117"/>
       <c r="M2" s="121" t="s">
+        <v>247</v>
+      </c>
+      <c r="N2" s="121" t="s">
         <v>248</v>
-      </c>
-      <c r="N2" s="121" t="s">
-        <v>249</v>
       </c>
       <c r="O2" s="120"/>
       <c r="P2" s="120"/>
@@ -15530,19 +15530,19 @@
         <v>42</v>
       </c>
       <c r="J1" s="52" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K1" s="51" t="s">
         <v>43</v>
       </c>
       <c r="L1" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M1" s="52" t="s">
         <v>133</v>
       </c>
       <c r="N1" s="52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O1" s="52" t="s">
         <v>140</v>
@@ -15551,10 +15551,10 @@
         <v>141</v>
       </c>
       <c r="Q1" s="52" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="R1" s="52" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S1" s="51" t="s">
         <v>3</v>
@@ -15607,7 +15607,7 @@
       <c r="Q2" s="128"/>
       <c r="R2" s="128"/>
       <c r="S2" s="124" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:44" ht="13" x14ac:dyDescent="0.15">
@@ -19269,7 +19269,7 @@
         <v>112</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>2</v>
@@ -19280,7 +19280,7 @@
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="130" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B2" s="131"/>
       <c r="C2" s="132"/>
@@ -19288,7 +19288,7 @@
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="130" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B3" s="134"/>
       <c r="C3" s="132"/>

</xml_diff>